<commit_message>
premier league - atualização de dados
atualizando rodada 5 do sabado - 22 de setembro
</commit_message>
<xml_diff>
--- a/premier_league_analise_cartoes_arquivo_de_saida.xlsx
+++ b/premier_league_analise_cartoes_arquivo_de_saida.xlsx
@@ -526,16 +526,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -547,10 +547,10 @@
         <v>3.5</v>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J3" t="n">
-        <v>2.25</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="4">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
@@ -572,19 +572,19 @@
         <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="I4" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="5">
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
         <v>2</v>
@@ -606,19 +606,19 @@
         <v>1.5</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" t="n">
-        <v>2</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="I5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J5" t="n">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="6">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>2</v>
@@ -674,19 +674,19 @@
         <v>2.5</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H7" t="n">
-        <v>5.5</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="I7" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J7" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="8">
@@ -730,16 +730,16 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
       <c r="E9" t="n">
-        <v>0.5</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
@@ -751,10 +751,10 @@
         <v>3.5</v>
       </c>
       <c r="I9" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J9" t="n">
-        <v>2</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="10">
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
         <v>2</v>
@@ -776,19 +776,19 @@
         <v>1.5</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J10" t="n">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="11">
@@ -798,16 +798,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="F11" t="n">
         <v>2</v>
@@ -819,10 +819,10 @@
         <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J11" t="n">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="12">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
         <v>2</v>
@@ -844,19 +844,19 @@
         <v>2.5</v>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H12" t="n">
-        <v>3</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="I12" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J12" t="n">
-        <v>2.75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -866,16 +866,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
         <v>2</v>
@@ -887,10 +887,10 @@
         <v>2.5</v>
       </c>
       <c r="I13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J13" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="14">
@@ -900,16 +900,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
@@ -921,10 +921,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="15">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
         <v>2</v>
@@ -946,19 +946,19 @@
         <v>3</v>
       </c>
       <c r="F15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H15" t="n">
-        <v>3</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="I15" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J15" t="n">
-        <v>3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="16">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
         <v>2</v>
@@ -980,19 +980,19 @@
         <v>3</v>
       </c>
       <c r="F16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G16" t="n">
         <v>5</v>
       </c>
       <c r="H16" t="n">
-        <v>2.5</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="I16" t="n">
         <v>11</v>
       </c>
       <c r="J16" t="n">
-        <v>2.75</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="17">
@@ -1036,16 +1036,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="F18" t="n">
         <v>2</v>
@@ -1057,10 +1057,10 @@
         <v>2.5</v>
       </c>
       <c r="I18" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J18" t="n">
-        <v>2.25</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="19">
@@ -1070,16 +1070,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E19" t="n">
-        <v>2.5</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="F19" t="n">
         <v>2</v>
@@ -1091,10 +1091,10 @@
         <v>2.5</v>
       </c>
       <c r="I19" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J19" t="n">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="20">
@@ -1104,16 +1104,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>2</v>
@@ -1125,10 +1125,10 @@
         <v>2</v>
       </c>
       <c r="I20" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J20" t="n">
-        <v>2</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="21">
@@ -1138,7 +1138,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
         <v>2</v>
@@ -1150,19 +1150,19 @@
         <v>2.5</v>
       </c>
       <c r="F21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I21" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J21" t="n">
-        <v>2.75</v>
+        <v>3.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualização da rodada 7
Rodada 7 da premier league
</commit_message>
<xml_diff>
--- a/premier_league_analise_cartoes_arquivo_de_saida.xlsx
+++ b/premier_league_analise_cartoes_arquivo_de_saida.xlsx
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>2.333333333333333</v>
+        <v>1.75</v>
       </c>
       <c r="F2" t="n">
         <v>3</v>
@@ -516,7 +516,7 @@
         <v>17</v>
       </c>
       <c r="J2" t="n">
-        <v>2.833333333333333</v>
+        <v>2.428571428571428</v>
       </c>
     </row>
     <row r="3">
@@ -526,16 +526,16 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5</v>
-      </c>
       <c r="E3" t="n">
-        <v>1.666666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="F3" t="n">
         <v>3</v>
@@ -547,10 +547,10 @@
         <v>2.666666666666667</v>
       </c>
       <c r="I3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J3" t="n">
-        <v>2.166666666666667</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -572,19 +572,19 @@
         <v>3.333333333333333</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" t="n">
-        <v>2.666666666666667</v>
+        <v>2.25</v>
       </c>
       <c r="I4" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>2.714285714285714</v>
       </c>
     </row>
     <row r="5">
@@ -594,16 +594,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>1.666666666666667</v>
+        <v>1.75</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -615,10 +615,10 @@
         <v>1.666666666666667</v>
       </c>
       <c r="I5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J5" t="n">
-        <v>1.666666666666667</v>
+        <v>1.714285714285714</v>
       </c>
     </row>
     <row r="6">
@@ -628,16 +628,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>2.666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="F6" t="n">
         <v>3</v>
@@ -649,10 +649,10 @@
         <v>1.666666666666667</v>
       </c>
       <c r="I6" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J6" t="n">
-        <v>2.166666666666667</v>
+        <v>2.142857142857143</v>
       </c>
     </row>
     <row r="7">
@@ -662,16 +662,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>2.666666666666667</v>
+        <v>3.5</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
@@ -683,10 +683,10 @@
         <v>4.333333333333333</v>
       </c>
       <c r="I7" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J7" t="n">
-        <v>3.5</v>
+        <v>3.857142857142857</v>
       </c>
     </row>
     <row r="8">
@@ -696,16 +696,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>2.666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="F8" t="n">
         <v>3</v>
@@ -717,10 +717,10 @@
         <v>2.333333333333333</v>
       </c>
       <c r="I8" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J8" t="n">
-        <v>2.5</v>
+        <v>2.428571428571428</v>
       </c>
     </row>
     <row r="9">
@@ -730,16 +730,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>1.333333333333333</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>3</v>
@@ -751,10 +751,10 @@
         <v>2.333333333333333</v>
       </c>
       <c r="I9" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J9" t="n">
-        <v>1.833333333333333</v>
+        <v>2.142857142857143</v>
       </c>
     </row>
     <row r="10">
@@ -764,16 +764,16 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
         <v>6</v>
       </c>
-      <c r="C10" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" t="n">
-        <v>5</v>
-      </c>
       <c r="E10" t="n">
-        <v>1.666666666666667</v>
+        <v>1.5</v>
       </c>
       <c r="F10" t="n">
         <v>3</v>
@@ -785,10 +785,10 @@
         <v>2</v>
       </c>
       <c r="I10" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J10" t="n">
-        <v>1.833333333333333</v>
+        <v>1.714285714285714</v>
       </c>
     </row>
     <row r="11">
@@ -798,7 +798,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
         <v>3</v>
@@ -810,19 +810,19 @@
         <v>3.333333333333333</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" t="n">
-        <v>3.333333333333333</v>
+        <v>2.75</v>
       </c>
       <c r="I11" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J11" t="n">
-        <v>3.333333333333333</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
         <v>3</v>
@@ -844,19 +844,19 @@
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" t="n">
-        <v>3.333333333333333</v>
+        <v>2.75</v>
       </c>
       <c r="I12" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" t="n">
-        <v>3.166666666666667</v>
+        <v>2.857142857142857</v>
       </c>
     </row>
     <row r="13">
@@ -866,16 +866,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F13" t="n">
         <v>3</v>
@@ -887,10 +887,10 @@
         <v>3</v>
       </c>
       <c r="I13" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J13" t="n">
-        <v>2.5</v>
+        <v>2.714285714285714</v>
       </c>
     </row>
     <row r="14">
@@ -900,7 +900,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" t="n">
         <v>3</v>
@@ -912,16 +912,16 @@
         <v>2.333333333333333</v>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G14" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H14" t="n">
-        <v>1.666666666666667</v>
+        <v>1.75</v>
       </c>
       <c r="I14" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J14" t="n">
         <v>2</v>
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" t="n">
         <v>3</v>
@@ -946,19 +946,19 @@
         <v>3.666666666666667</v>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H15" t="n">
-        <v>2.666666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="I15" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J15" t="n">
-        <v>3.166666666666667</v>
+        <v>3.428571428571428</v>
       </c>
     </row>
     <row r="16">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" t="n">
         <v>3</v>
@@ -980,19 +980,19 @@
         <v>3.333333333333333</v>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H16" t="n">
-        <v>1.666666666666667</v>
+        <v>1.75</v>
       </c>
       <c r="I16" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J16" t="n">
-        <v>2.5</v>
+        <v>2.428571428571428</v>
       </c>
     </row>
     <row r="17">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" t="n">
         <v>3</v>
@@ -1014,19 +1014,19 @@
         <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G17" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H17" t="n">
-        <v>3.666666666666667</v>
+        <v>3.25</v>
       </c>
       <c r="I17" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J17" t="n">
-        <v>2.833333333333333</v>
+        <v>2.714285714285714</v>
       </c>
     </row>
     <row r="18">
@@ -1036,7 +1036,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" t="n">
         <v>3</v>
@@ -1048,16 +1048,16 @@
         <v>2.666666666666667</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G18" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H18" t="n">
-        <v>3.333333333333333</v>
+        <v>3.25</v>
       </c>
       <c r="I18" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="J18" t="n">
         <v>3</v>
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
         <v>3</v>
@@ -1082,19 +1082,19 @@
         <v>2.666666666666667</v>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G19" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H19" t="n">
-        <v>2.666666666666667</v>
+        <v>2.5</v>
       </c>
       <c r="I19" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J19" t="n">
-        <v>2.666666666666667</v>
+        <v>2.571428571428572</v>
       </c>
     </row>
     <row r="20">
@@ -1104,16 +1104,16 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" t="n">
         <v>9</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="F20" t="n">
         <v>3</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="J20" t="n">
-        <v>2.666666666666667</v>
+        <v>2.285714285714286</v>
       </c>
     </row>
     <row r="21">
@@ -1138,7 +1138,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" t="n">
         <v>3</v>
@@ -1150,19 +1150,19 @@
         <v>2.333333333333333</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="I21" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="J21" t="n">
-        <v>3.166666666666667</v>
+        <v>3.142857142857143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>